<commit_message>
Update results with new corpus
</commit_message>
<xml_diff>
--- a/resources/annotated_java_test.xlsx
+++ b/resources/annotated_java_test.xlsx
@@ -1,23 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilapaiva/Documents/GitHub/db-mining/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Planilha1!$A$1:$W$2</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>owner</t>
   </si>
@@ -139,6 +152,15 @@
     <t>APM, Application Performance Monitoring System</t>
   </si>
   <si>
+    <t>camel</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>http://www.github.com/apache/camel</t>
+  </si>
+  <si>
     <t>storm</t>
   </si>
   <si>
@@ -149,16 +171,46 @@
   </si>
   <si>
     <t>Mirror of Apache Storm</t>
+  </si>
+  <si>
+    <t>oracle</t>
+  </si>
+  <si>
+    <t>graal</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>http://www.github.com/oracle/graal</t>
+  </si>
+  <si>
+    <t>GraalVM: Run Programs Faster Anywhere :rocket:</t>
+  </si>
+  <si>
+    <t>Software Development</t>
+  </si>
+  <si>
+    <t>RoaringBitmap</t>
+  </si>
+  <si>
+    <t>http://www.github.com/RoaringBitmap/RoaringBitmap</t>
+  </si>
+  <si>
+    <t>A better compressed bitset in Java</t>
+  </si>
+  <si>
+    <t>Data Management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,12 +226,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -187,15 +233,36 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF0000ff"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -209,7 +276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFb7e1cd"/>
+        <fgColor rgb="FFB7E1CD"/>
       </patternFill>
     </fill>
   </fills>
@@ -245,88 +312,78 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -337,10 +394,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -378,71 +435,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -470,7 +527,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -493,11 +550,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -506,13 +563,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -522,7 +579,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -531,7 +588,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -540,7 +597,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -548,10 +605,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -617,41 +674,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" style="15" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="18" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="18" width="5.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="18" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="18" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="18" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="18" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="18" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="18" width="7.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="15" width="32.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="17" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="17" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="17" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="15" width="255.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="6.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="255.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,352 +781,565 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5">
-        <v>41165.48244212963</v>
-      </c>
-      <c r="D2" s="5">
-        <v>43700.5015162037</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="7">
+        <v>41165.482442129629</v>
+      </c>
+      <c r="D2" s="7">
+        <v>43700.501516203702</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="8">
         <v>95935</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="8">
         <v>5</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="8">
         <v>171</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="8">
         <v>623</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="8">
         <v>5618</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="8">
         <v>4634</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="8">
         <v>1456</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="8">
         <v>8458</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="8">
         <v>1411</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="8">
         <v>74</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="8">
         <v>263</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="8">
         <v>23</v>
       </c>
-      <c r="S2" s="7">
+      <c r="S2" s="4" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A2),"/"),B2)</f>
-      </c>
-      <c r="T2" s="8" t="s">
+        <v>http://www.github.com/Activiti/Activiti</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="5">
-        <v>42089.64653935185</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="7">
+        <v>42089.646539351852</v>
+      </c>
+      <c r="D3" s="7">
         <v>43700.588159722225</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="8">
         <v>128730</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="8">
         <v>19</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="8">
         <v>136</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="8">
         <v>322</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="8">
         <v>5651</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="8">
         <v>1053</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="8">
         <v>8160</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="8">
         <v>8103</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="8">
         <v>6158</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="8">
         <v>58</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="8">
         <v>150</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="8">
         <v>12</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="4" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A3),"/"),B3)</f>
-      </c>
-      <c r="T3" s="8" t="s">
+        <v>http://www.github.com/eclipse/che</v>
+      </c>
+      <c r="T3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4" t="s">
+      <c r="U3" s="6"/>
+      <c r="V3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="11">
-        <v>41932.39400462963</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="C4" s="7">
+        <v>41932.394004629627</v>
+      </c>
+      <c r="D4" s="7">
         <v>43700.351875</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="8">
         <v>220959</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="8">
         <v>15</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="8">
         <v>75</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="8">
         <v>793</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="8">
         <v>9204</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="8">
         <v>2815</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="8">
         <v>2355</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="8">
         <v>10643</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="8">
         <v>3553</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="8">
         <v>8</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="8">
         <v>30</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="8">
         <v>30</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="10" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A4),"/"),B4)</f>
-      </c>
-      <c r="T4" s="10" t="s">
+        <v>http://www.github.com/naver/pinpoint</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10" t="s">
+      <c r="U4" s="6"/>
+      <c r="V4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="W4" s="14" t="s">
+      <c r="W4" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5">
-        <v>42315.14625</v>
-      </c>
-      <c r="D5" s="5">
-        <v>43700.44155092593</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="7">
+        <v>42315.146249999998</v>
+      </c>
+      <c r="D5" s="7">
+        <v>43700.441550925927</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="8">
         <v>145291</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="8">
         <v>9</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="8">
         <v>168</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="8">
         <v>702</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="8">
         <v>9980</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="8">
         <v>2866</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="8">
         <v>1558</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="8">
         <v>5039</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="8">
         <v>1748</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="8">
         <v>9</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="8">
         <v>34</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="8">
         <v>33</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="4" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A5),"/"),B5)</f>
-      </c>
-      <c r="T5" s="8" t="s">
+        <v>http://www.github.com/apache/skywalking</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4" t="s">
+      <c r="U5" s="6"/>
+      <c r="V5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="5">
-        <v>41583.33349537037</v>
-      </c>
-      <c r="D6" s="5">
-        <v>43700.34212962963</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="11">
+        <v>39954.017777777779</v>
+      </c>
+      <c r="D6" s="11">
+        <v>43700.054328703707</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="12">
+        <v>294421</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="12">
+        <v>16</v>
+      </c>
+      <c r="I6" s="12">
+        <v>526</v>
+      </c>
+      <c r="J6" s="12">
+        <v>288</v>
+      </c>
+      <c r="K6" s="12">
+        <v>2793</v>
+      </c>
+      <c r="L6" s="12">
+        <v>3640</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>39167</v>
+      </c>
+      <c r="O6" s="12">
+        <v>3104</v>
+      </c>
+      <c r="P6" s="12">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>145</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="7">
+        <v>41583.333495370367</v>
+      </c>
+      <c r="D7" s="7">
+        <v>43700.342129629629</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="8">
         <v>179069</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H7" s="8">
         <v>16</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I7" s="8">
         <v>338</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J7" s="8">
         <v>633</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K7" s="8">
         <v>5812</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L7" s="8">
         <v>3940</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M7" s="8">
         <v>0</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N7" s="8">
         <v>10100</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O7" s="8">
         <v>3116</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P7" s="8">
         <v>39</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q7" s="8">
         <v>40</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R7" s="8">
         <v>0</v>
       </c>
-      <c r="S6" s="7">
-        <f>concatenate(concatenate(concatenate("http://www.github.com/", A6), "/"), B6)</f>
-      </c>
-      <c r="T6" s="8" t="s">
+      <c r="S7" s="4" t="str">
+        <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/", A7), "/"), B7)</f>
+        <v>http://www.github.com/apache/storm</v>
+      </c>
+      <c r="T7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="W6" s="9" t="s">
-        <v>43</v>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="13">
+        <v>42383.716377314813</v>
+      </c>
+      <c r="D8" s="13">
+        <v>43700.545902777776</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="5">
+        <v>799868</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5">
+        <v>15</v>
+      </c>
+      <c r="I8" s="5">
+        <v>139</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1697</v>
+      </c>
+      <c r="K8" s="5">
+        <v>403</v>
+      </c>
+      <c r="L8" s="5">
+        <v>10070</v>
+      </c>
+      <c r="M8" s="5">
+        <v>19962</v>
+      </c>
+      <c r="N8" s="5">
+        <v>648</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1597</v>
+      </c>
+      <c r="P8" s="5">
+        <v>1147</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>37550</v>
+      </c>
+      <c r="R8" s="5">
+        <v>83468</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="13">
+        <v>41442.853738425925</v>
+      </c>
+      <c r="D9" s="13">
+        <v>43678.040983796294</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="5">
+        <v>85477</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5</v>
+      </c>
+      <c r="I9" s="5">
+        <v>56</v>
+      </c>
+      <c r="J9" s="5">
+        <v>90</v>
+      </c>
+      <c r="K9" s="5">
+        <v>102</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1381</v>
+      </c>
+      <c r="M9" s="5">
+        <v>3439</v>
+      </c>
+      <c r="N9" s="5">
+        <v>261</v>
+      </c>
+      <c r="O9" s="5">
+        <v>540</v>
+      </c>
+      <c r="P9" s="5">
+        <v>189</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>1925</v>
+      </c>
+      <c r="R9" s="5">
+        <v>2382</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S8" r:id="rId1"/>
+    <hyperlink ref="S9" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Results and analise dfs
</commit_message>
<xml_diff>
--- a/resources/annotated_java_test.xlsx
+++ b/resources/annotated_java_test.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>owner</t>
   </si>
@@ -207,6 +207,63 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>jchambers</t>
+  </si>
+  <si>
+    <t>pushy</t>
+  </si>
+  <si>
+    <t>http://www.github.com/jchambers/pushy</t>
+  </si>
+  <si>
+    <t>A Java library for sending APNs (iOS/macOS/Safari) push notifications</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>RoaringBitmap</t>
+  </si>
+  <si>
+    <t>http://www.github.com/RoaringBitmap/RoaringBitmap</t>
+  </si>
+  <si>
+    <t>Data Management</t>
+  </si>
+  <si>
+    <t>nextcloud</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>http://www.github.com/nextcloud/android</t>
+  </si>
+  <si>
+    <t>File Management</t>
+  </si>
+  <si>
+    <t>cSploit</t>
+  </si>
+  <si>
+    <t>http://www.github.com/cSploit/android</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>AntennaPod</t>
+  </si>
+  <si>
+    <t>http://www.github.com/AntennaPod/AntennaPod</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -341,62 +398,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -700,19 +725,19 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" style="12" bestFit="1" customWidth="1"/>
@@ -724,15 +749,15 @@
     <col min="16" max="16" width="8.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="44" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="94.83203125" style="5" customWidth="1"/>
-    <col min="24" max="16384" width="8.83203125" style="5"/>
+    <col min="19" max="19" width="44" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="94.83203125" style="4" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,299 +828,299 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>41165.482442129629</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>43700.501516203702</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>95935</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>5</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>171</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>623</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <v>5618</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <v>4634</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="7">
         <v>1456</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="7">
         <v>8458</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="7">
         <v>1411</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="7">
         <v>74</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="7">
         <v>263</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R2" s="7">
         <v>23</v>
       </c>
-      <c r="S2" s="4" t="str">
+      <c r="S2" s="8" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A2),"/"),B2)</f>
         <v>http://www.github.com/Activiti/Activiti</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>42089.646539351852</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>43700.588159722225</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>128730</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>19</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>136</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>322</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>5651</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>1053</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="7">
         <v>8160</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>8103</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>6158</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="7">
         <v>58</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="7">
         <v>150</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3" s="7">
         <v>12</v>
       </c>
-      <c r="S3" s="4" t="str">
+      <c r="S3" s="8" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A3),"/"),B3)</f>
         <v>http://www.github.com/eclipse/che</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>41932.394004629627</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>43700.351875</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>220959</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>15</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>75</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>793</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <v>9204</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <v>2815</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="7">
         <v>2355</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <v>10643</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>3553</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="7">
         <v>8</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="7">
         <v>30</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4" s="7">
         <v>30</v>
       </c>
       <c r="S4" s="10" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A4),"/"),B4)</f>
         <v>http://www.github.com/naver/pinpoint</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="V4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="W4" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>42315.146249999998</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>43700.441550925927</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>145291</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>9</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>168</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <v>702</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>9980</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="7">
         <v>2866</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="7">
         <v>1558</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <v>5039</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <v>1748</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="7">
         <v>9</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="7">
         <v>34</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="7">
         <v>33</v>
       </c>
-      <c r="S5" s="4" t="str">
+      <c r="S5" s="8" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A5),"/"),B5)</f>
         <v>http://www.github.com/apache/skywalking</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="V5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="11">
@@ -1104,13 +1129,13 @@
       <c r="D6" s="11">
         <v>43700.054328703707</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="12">
         <v>294421</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="12">
@@ -1146,99 +1171,99 @@
       <c r="R6" s="12">
         <v>0</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="T6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="U6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="W6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>41583.333495370367</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>43700.342129629629</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>179069</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>16</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>338</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>633</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>5812</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>3940</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>0</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>10100</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <v>3116</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="7">
         <v>39</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="7">
         <v>40</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7" s="7">
         <v>0</v>
       </c>
-      <c r="S7" s="4" t="str">
+      <c r="S7" s="8" t="str">
         <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/", A7), "/"), B7)</f>
         <v>http://www.github.com/apache/storm</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="U7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="V7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="13">
@@ -1247,62 +1272,65 @@
       <c r="D8" s="13">
         <v>43700.545902777776</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>799868</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>15</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>139</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>1697</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>403</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>10070</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>19962</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <v>648</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="4">
         <v>1597</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="4">
         <v>1147</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="4">
         <v>37550</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="4">
         <v>83468</v>
       </c>
       <c r="S8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="T8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="U8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="W8" s="5" t="s">
+      <c r="W8" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>53</v>
       </c>
@@ -1360,26 +1388,381 @@
       <c r="S9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="T9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U9" s="18"/>
+      <c r="U9" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="V9" s="18" t="s">
         <v>57</v>
       </c>
       <c r="W9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="X9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
+    </row>
+    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="16">
+        <v>41488.818414351852</v>
+      </c>
+      <c r="D10" s="16">
+        <v>44270.661932870367</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="15">
+        <v>7908</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="15">
+        <v>4</v>
+      </c>
+      <c r="I10" s="15">
+        <v>34</v>
+      </c>
+      <c r="J10" s="15">
+        <v>41</v>
+      </c>
+      <c r="K10" s="15">
+        <v>168</v>
+      </c>
+      <c r="L10" s="15">
+        <v>1358</v>
+      </c>
+      <c r="M10" s="15">
+        <v>1778</v>
+      </c>
+      <c r="N10" s="15">
+        <v>368</v>
+      </c>
+      <c r="O10" s="15">
+        <v>448</v>
+      </c>
+      <c r="P10" s="15">
+        <v>528</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>1522</v>
+      </c>
+      <c r="R10" s="15">
+        <v>1598</v>
+      </c>
+      <c r="S10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V10" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="20">
+        <v>41442.853738425925</v>
+      </c>
+      <c r="D11" s="20">
+        <v>43678.040983796294</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="19">
+        <v>85477</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="19">
+        <v>5</v>
+      </c>
+      <c r="I11" s="19">
+        <v>56</v>
+      </c>
+      <c r="J11" s="19">
+        <v>90</v>
+      </c>
+      <c r="K11" s="19">
+        <v>102</v>
+      </c>
+      <c r="L11" s="19">
+        <v>1381</v>
+      </c>
+      <c r="M11" s="19">
+        <v>3439</v>
+      </c>
+      <c r="N11" s="19">
+        <v>261</v>
+      </c>
+      <c r="O11" s="19">
+        <v>540</v>
+      </c>
+      <c r="P11" s="19">
+        <v>189</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>1925</v>
+      </c>
+      <c r="R11" s="19">
+        <v>2382</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="20">
+        <v>42527.891388888886</v>
+      </c>
+      <c r="D12" s="20">
+        <v>43700.347361111111</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="19">
+        <v>378332</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="19">
+        <v>8</v>
+      </c>
+      <c r="I12" s="19">
+        <v>240</v>
+      </c>
+      <c r="J12" s="19">
+        <v>395</v>
+      </c>
+      <c r="K12" s="19">
+        <v>144</v>
+      </c>
+      <c r="L12" s="19">
+        <v>1425</v>
+      </c>
+      <c r="M12" s="19">
+        <v>4033</v>
+      </c>
+      <c r="N12" s="19">
+        <v>720</v>
+      </c>
+      <c r="O12" s="19">
+        <v>1736</v>
+      </c>
+      <c r="P12" s="19">
+        <v>2468</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>13282</v>
+      </c>
+      <c r="R12" s="19">
+        <v>24286</v>
+      </c>
+      <c r="S12" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V12" t="s">
+        <v>70</v>
+      </c>
+      <c r="W12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="20">
+        <v>41916.245474537034</v>
+      </c>
+      <c r="D13" s="20">
+        <v>43683.769004629627</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="19">
+        <v>39599</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="19">
+        <v>2</v>
+      </c>
+      <c r="I13" s="19">
+        <v>56</v>
+      </c>
+      <c r="J13" s="19">
+        <v>56</v>
+      </c>
+      <c r="K13" s="19">
+        <v>349</v>
+      </c>
+      <c r="L13" s="19">
+        <v>2261</v>
+      </c>
+      <c r="M13" s="19">
+        <v>3260</v>
+      </c>
+      <c r="N13" s="19">
+        <v>951</v>
+      </c>
+      <c r="O13" s="19">
+        <v>1097</v>
+      </c>
+      <c r="P13" s="19">
+        <v>861</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>1403</v>
+      </c>
+      <c r="R13" s="19">
+        <v>1405</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="20">
+        <v>41121.434120370373</v>
+      </c>
+      <c r="D14" s="20">
+        <v>43700.328738425924</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="19">
+        <v>33200</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="19">
+        <v>4</v>
+      </c>
+      <c r="I14" s="19">
+        <v>113</v>
+      </c>
+      <c r="J14" s="19">
+        <v>255</v>
+      </c>
+      <c r="K14" s="19">
+        <v>159</v>
+      </c>
+      <c r="L14" s="19">
+        <v>2442</v>
+      </c>
+      <c r="M14" s="19">
+        <v>6031</v>
+      </c>
+      <c r="N14" s="19">
+        <v>732</v>
+      </c>
+      <c r="O14" s="19">
+        <v>1368</v>
+      </c>
+      <c r="P14" s="19">
+        <v>2058</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>5171</v>
+      </c>
+      <c r="R14" s="19">
+        <v>8871</v>
+      </c>
+      <c r="S14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="T14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14"/>
+      <c r="V14" t="s">
+        <v>76</v>
+      </c>
+      <c r="W14" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="S8" r:id="rId1"/>
     <hyperlink ref="S9" r:id="rId2"/>
+    <hyperlink ref="S10" r:id="rId3"/>
+    <hyperlink ref="S11" r:id="rId4"/>
+    <hyperlink ref="S12" r:id="rId5"/>
+    <hyperlink ref="S13" r:id="rId6"/>
+    <hyperlink ref="S14" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>